<commit_message>
Introdução PT + Cronograma atualizado
</commit_message>
<xml_diff>
--- a/Cronograma-PAP.xlsx
+++ b/Cronograma-PAP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28646380-F7A8-4CF2-9DA8-759A876BA00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C568F3-17FA-4916-A168-0448E7985254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="16530" tabRatio="476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="12960" tabRatio="476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12º Ano" sheetId="3" r:id="rId1"/>
@@ -117,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +168,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,30 +392,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -423,6 +406,31 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,8 +439,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4472C4"/>
       <color rgb="FFF40CC8"/>
-      <color rgb="FF4472C4"/>
     </mruColors>
   </colors>
   <extLst>
@@ -735,331 +743,331 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection sqref="A1:AU20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.7265625" customWidth="1"/>
-    <col min="3" max="42" width="4.7265625" customWidth="1"/>
-    <col min="43" max="43" width="5.1796875" customWidth="1"/>
-    <col min="44" max="44" width="4.7265625" customWidth="1"/>
-    <col min="45" max="46" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="42" width="4.7109375" customWidth="1"/>
+    <col min="43" max="43" width="5.140625" customWidth="1"/>
+    <col min="44" max="44" width="4.7109375" customWidth="1"/>
+    <col min="45" max="46" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:47" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="11"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="27"/>
+      <c r="AQ1" s="27"/>
+      <c r="AR1" s="27"/>
+      <c r="AS1" s="27"/>
+      <c r="AT1" s="28"/>
       <c r="AU1" s="1"/>
     </row>
-    <row r="2" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12" t="s">
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12" t="s">
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12" t="s">
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12" t="s">
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12" t="s">
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="12" t="s">
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="12" t="s">
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12" t="s">
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+      <c r="AQ2" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="12"/>
+      <c r="AR2" s="23"/>
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="23"/>
       <c r="AU2" s="1"/>
     </row>
-    <row r="3" spans="1:47" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:47" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="21">
         <v>1</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="21">
         <v>2</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="21">
         <v>3</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="21">
         <v>4</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="21">
         <v>1</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="21">
         <v>2</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="21">
         <v>3</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="21">
         <v>4</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="21">
         <v>1</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="21">
         <v>2</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="21">
         <v>3</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="21">
         <v>4</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="21">
         <v>1</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="21">
         <v>2</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="21">
         <v>3</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="21">
         <v>4</v>
       </c>
-      <c r="S3" s="7">
+      <c r="S3" s="21">
         <v>1</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="21">
         <v>2</v>
       </c>
-      <c r="U3" s="7">
+      <c r="U3" s="21">
         <v>3</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="21">
         <v>4</v>
       </c>
-      <c r="W3" s="7">
+      <c r="W3" s="21">
         <v>1</v>
       </c>
-      <c r="X3" s="7">
+      <c r="X3" s="21">
         <v>2</v>
       </c>
-      <c r="Y3" s="7">
+      <c r="Y3" s="21">
         <v>3</v>
       </c>
-      <c r="Z3" s="7">
+      <c r="Z3" s="21">
         <v>4</v>
       </c>
-      <c r="AA3" s="7">
+      <c r="AA3" s="21">
         <v>1</v>
       </c>
-      <c r="AB3" s="7">
+      <c r="AB3" s="21">
         <v>2</v>
       </c>
-      <c r="AC3" s="7">
+      <c r="AC3" s="21">
         <v>3</v>
       </c>
-      <c r="AD3" s="7">
+      <c r="AD3" s="21">
         <v>4</v>
       </c>
-      <c r="AE3" s="7">
+      <c r="AE3" s="21">
         <v>1</v>
       </c>
-      <c r="AF3" s="7">
+      <c r="AF3" s="21">
         <v>2</v>
       </c>
-      <c r="AG3" s="7">
+      <c r="AG3" s="21">
         <v>3</v>
       </c>
-      <c r="AH3" s="7">
+      <c r="AH3" s="21">
         <v>4</v>
       </c>
-      <c r="AI3" s="7">
+      <c r="AI3" s="21">
         <v>1</v>
       </c>
-      <c r="AJ3" s="7">
+      <c r="AJ3" s="21">
         <v>2</v>
       </c>
-      <c r="AK3" s="7">
+      <c r="AK3" s="21">
         <v>3</v>
       </c>
-      <c r="AL3" s="7">
+      <c r="AL3" s="21">
         <v>4</v>
       </c>
-      <c r="AM3" s="7">
+      <c r="AM3" s="21">
         <v>1</v>
       </c>
-      <c r="AN3" s="7">
+      <c r="AN3" s="21">
         <v>2</v>
       </c>
-      <c r="AO3" s="7">
+      <c r="AO3" s="21">
         <v>3</v>
       </c>
-      <c r="AP3" s="7">
+      <c r="AP3" s="21">
         <v>4</v>
       </c>
-      <c r="AQ3" s="7">
+      <c r="AQ3" s="21">
         <v>1</v>
       </c>
-      <c r="AR3" s="7">
+      <c r="AR3" s="21">
         <v>2</v>
       </c>
-      <c r="AS3" s="7">
+      <c r="AS3" s="21">
         <v>3</v>
       </c>
-      <c r="AT3" s="7">
+      <c r="AT3" s="21">
         <v>4</v>
       </c>
       <c r="AU3" s="1"/>
     </row>
-    <row r="4" spans="1:47" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:47" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="8"/>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="8"/>
-      <c r="AN4" s="8"/>
-      <c r="AO4" s="8"/>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="8"/>
-      <c r="AR4" s="8"/>
-      <c r="AS4" s="8"/>
-      <c r="AT4" s="8"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="22"/>
+      <c r="AM4" s="22"/>
+      <c r="AN4" s="22"/>
+      <c r="AO4" s="22"/>
+      <c r="AP4" s="22"/>
+      <c r="AQ4" s="22"/>
+      <c r="AR4" s="22"/>
+      <c r="AS4" s="22"/>
+      <c r="AT4" s="22"/>
       <c r="AU4" s="1"/>
     </row>
-    <row r="5" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1111,18 +1119,18 @@
       <c r="AT5" s="3"/>
       <c r="AU5" s="1"/>
     </row>
-    <row r="6" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -1162,8 +1170,8 @@
       <c r="AT6" s="3"/>
       <c r="AU6" s="1"/>
     </row>
-    <row r="7" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1213,8 +1221,8 @@
       <c r="AT7" s="3"/>
       <c r="AU7" s="1"/>
     </row>
-    <row r="8" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1222,11 +1230,11 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -1264,12 +1272,12 @@
       <c r="AT8" s="3"/>
       <c r="AU8" s="1"/>
     </row>
-    <row r="9" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1277,22 +1285,22 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
@@ -1317,10 +1325,10 @@
       <c r="AT9" s="3"/>
       <c r="AU9" s="1"/>
     </row>
-    <row r="10" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1328,38 +1336,38 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-      <c r="AE10" s="20"/>
-      <c r="AF10" s="20"/>
-      <c r="AG10" s="20"/>
-      <c r="AH10" s="20"/>
-      <c r="AI10" s="20"/>
-      <c r="AJ10" s="20"/>
-      <c r="AK10" s="20"/>
-      <c r="AL10" s="20"/>
-      <c r="AM10" s="20"/>
-      <c r="AN10" s="20"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="12"/>
+      <c r="AJ10" s="12"/>
+      <c r="AK10" s="12"/>
+      <c r="AL10" s="12"/>
+      <c r="AM10" s="12"/>
+      <c r="AN10" s="12"/>
       <c r="AO10" s="3"/>
       <c r="AP10" s="3"/>
       <c r="AQ10" s="3"/>
@@ -1368,8 +1376,8 @@
       <c r="AT10" s="3"/>
       <c r="AU10" s="1"/>
     </row>
-    <row r="11" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1395,21 +1403,21 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
       <c r="AF11" s="3"/>
       <c r="AG11" s="5"/>
-      <c r="AI11" s="16"/>
+      <c r="AI11" s="8"/>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
       <c r="AL11" s="5"/>
       <c r="AM11" s="5"/>
-      <c r="AN11" s="16"/>
+      <c r="AN11" s="8"/>
       <c r="AO11" s="3"/>
       <c r="AP11" s="3"/>
       <c r="AQ11" s="3"/>
@@ -1418,8 +1426,8 @@
       <c r="AT11" s="3"/>
       <c r="AU11" s="1"/>
     </row>
-    <row r="12" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1439,30 +1447,30 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="17"/>
+      <c r="Q12" s="9"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
-      <c r="V12" s="17"/>
-      <c r="W12" s="16"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="8"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="17"/>
+      <c r="AB12" s="9"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
-      <c r="AF12" s="24"/>
+      <c r="AF12" s="16"/>
       <c r="AG12" s="3"/>
-      <c r="AH12" s="17"/>
+      <c r="AH12" s="9"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
       <c r="AM12" s="3"/>
-      <c r="AN12" s="17"/>
+      <c r="AN12" s="9"/>
       <c r="AO12" s="3"/>
       <c r="AP12" s="3"/>
       <c r="AQ12" s="3"/>
@@ -1471,8 +1479,8 @@
       <c r="AT12" s="3"/>
       <c r="AU12" s="1"/>
     </row>
-    <row r="13" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1502,10 +1510,10 @@
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
-      <c r="AC13" s="22"/>
-      <c r="AD13" s="22"/>
-      <c r="AE13" s="22"/>
-      <c r="AF13" s="22"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="14"/>
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
@@ -1522,8 +1530,8 @@
       <c r="AT13" s="3"/>
       <c r="AU13" s="1"/>
     </row>
-    <row r="14" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1557,12 +1565,12 @@
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
-      <c r="AG14" s="24"/>
+      <c r="AG14" s="16"/>
       <c r="AH14" s="3"/>
-      <c r="AI14" s="23"/>
-      <c r="AJ14" s="23"/>
-      <c r="AK14" s="23"/>
-      <c r="AL14" s="23"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+      <c r="AL14" s="15"/>
       <c r="AM14" s="3"/>
       <c r="AN14" s="3"/>
       <c r="AO14" s="3"/>
@@ -1573,7 +1581,7 @@
       <c r="AT14" s="3"/>
       <c r="AU14" s="1"/>
     </row>
-    <row r="15" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>27</v>
@@ -1581,41 +1589,41 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="25"/>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
-      <c r="AD15" s="25"/>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="25"/>
-      <c r="AH15" s="25"/>
-      <c r="AI15" s="25"/>
-      <c r="AJ15" s="25"/>
-      <c r="AK15" s="25"/>
-      <c r="AL15" s="25"/>
-      <c r="AM15" s="25"/>
-      <c r="AN15" s="25"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="17"/>
+      <c r="AH15" s="17"/>
+      <c r="AI15" s="17"/>
+      <c r="AJ15" s="17"/>
+      <c r="AK15" s="17"/>
+      <c r="AL15" s="17"/>
+      <c r="AM15" s="17"/>
+      <c r="AN15" s="17"/>
       <c r="AO15" s="3"/>
       <c r="AP15" s="3"/>
       <c r="AQ15" s="3"/>
@@ -1624,7 +1632,7 @@
       <c r="AT15" s="3"/>
       <c r="AU15" s="1"/>
     </row>
-    <row r="16" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>28</v>
@@ -1667,7 +1675,7 @@
       <c r="AL16" s="3"/>
       <c r="AM16" s="3"/>
       <c r="AN16" s="3"/>
-      <c r="AO16" s="26"/>
+      <c r="AO16" s="18"/>
       <c r="AP16" s="3"/>
       <c r="AQ16" s="3"/>
       <c r="AR16" s="3"/>
@@ -1675,7 +1683,7 @@
       <c r="AT16" s="3"/>
       <c r="AU16" s="1"/>
     </row>
-    <row r="17" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
         <v>13</v>
@@ -1719,14 +1727,14 @@
       <c r="AM17" s="3"/>
       <c r="AN17" s="3"/>
       <c r="AO17" s="3"/>
-      <c r="AP17" s="27"/>
-      <c r="AQ17" s="27"/>
+      <c r="AP17" s="19"/>
+      <c r="AQ17" s="19"/>
       <c r="AR17" s="3"/>
       <c r="AS17" s="3"/>
       <c r="AT17" s="3"/>
       <c r="AU17" s="1"/>
     </row>
-    <row r="18" spans="1:47" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
         <v>29</v>
@@ -1772,12 +1780,12 @@
       <c r="AO18" s="3"/>
       <c r="AP18" s="3"/>
       <c r="AQ18" s="3"/>
-      <c r="AR18" s="28"/>
+      <c r="AR18" s="20"/>
       <c r="AS18" s="3"/>
       <c r="AT18" s="3"/>
       <c r="AU18" s="1"/>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1826,7 +1834,7 @@
       <c r="AT19" s="1"/>
       <c r="AU19" s="1"/>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1877,18 +1885,38 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AN3:AN4"/>
-    <mergeCell ref="AO3:AO4"/>
-    <mergeCell ref="AP3:AP4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="C1:AT1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AR3:AR4"/>
+    <mergeCell ref="AS3:AS4"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="AD3:AD4"/>
@@ -1905,38 +1933,18 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="C1:AT1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AR3:AR4"/>
-    <mergeCell ref="AS3:AS4"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AN3:AN4"/>
+    <mergeCell ref="AO3:AO4"/>
+    <mergeCell ref="AP3:AP4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>